<commit_message>
Add test to confirm duplicates are not getting created
</commit_message>
<xml_diff>
--- a/spec/support/files/2010_analyzed_mesh_terms.xlsx
+++ b/spec/support/files/2010_analyzed_mesh_terms.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="79">
   <si>
     <t>A Pulmonary Term</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -307,6 +307,12 @@
   <si>
     <t>N</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C21.866.915.300.200.150</t>
+  </si>
+  <si>
+    <t>Brain Concussion</t>
   </si>
 </sst>
 </file>
@@ -731,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A26" sqref="A26:Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="13"/>
@@ -2081,6 +2087,59 @@
         <v>27</v>
       </c>
     </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P26" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>